<commit_message>
Added runtimes for fixed dataset size and varying smote parameters
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VCU\CMSC635\Project\BorderlineSMOTE-Experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92674AF4-3B62-4B51-B38B-F3C275E41A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6626CD18-B7DC-4153-85AA-CABEF305839C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="13">
   <si>
     <t>Unsampled</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Before Sampling</t>
+  </si>
+  <si>
+    <t>Runtime (s)</t>
   </si>
 </sst>
 </file>
@@ -388,18 +391,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I69" sqref="I69"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -408,7 +412,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -422,8 +426,11 @@
       <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C3">
         <v>0.88370000000000004</v>
       </c>
@@ -436,8 +443,11 @@
       <c r="F3">
         <v>0.84289999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>3.0109384059906001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -447,7 +457,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -463,8 +473,11 @@
       <c r="F6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -480,8 +493,11 @@
       <c r="F7">
         <v>0.83919999999999995</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>2.1193897724151598</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
@@ -497,8 +513,11 @@
       <c r="F8">
         <v>0.84279999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>2.0937805175781201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10</v>
       </c>
@@ -514,8 +533,11 @@
       <c r="F9">
         <v>0.83499999999999996</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>2.1435699462890598</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>15</v>
       </c>
@@ -531,8 +553,11 @@
       <c r="F10">
         <v>0.83989999999999998</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>2.162353515625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>20</v>
       </c>
@@ -548,8 +573,11 @@
       <c r="F11">
         <v>0.84660000000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>2.22353911399841</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -570,7 +598,7 @@
         <v>0.84660000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -580,7 +608,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -599,8 +627,11 @@
       <c r="F15" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -619,8 +650,11 @@
       <c r="F16">
         <v>0.85229999999999995</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <v>2.2552626132964999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -639,8 +673,11 @@
       <c r="F17">
         <v>0.84409999999999996</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17">
+        <v>2.5098481178283598</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -659,8 +696,11 @@
       <c r="F18">
         <v>0.84260000000000002</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <v>2.8897750377654998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -679,8 +719,11 @@
       <c r="F19">
         <v>0.8407</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <v>3.09475350379943</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -699,8 +742,11 @@
       <c r="F20">
         <v>0.84299999999999997</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20">
+        <v>3.2664694786071702</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>5</v>
       </c>
@@ -719,8 +765,11 @@
       <c r="F21">
         <v>0.85140000000000005</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21">
+        <v>2.2354357242584202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>5</v>
       </c>
@@ -739,8 +788,11 @@
       <c r="F22">
         <v>0.84150000000000003</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22">
+        <v>2.5341119766235298</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>5</v>
       </c>
@@ -759,8 +811,11 @@
       <c r="F23">
         <v>0.84289999999999998</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23">
+        <v>2.9711067676544101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>5</v>
       </c>
@@ -779,8 +834,11 @@
       <c r="F24">
         <v>0.83850000000000002</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <v>3.09894371032714</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>5</v>
       </c>
@@ -799,8 +857,11 @@
       <c r="F25">
         <v>0.83709999999999996</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <v>3.2883157730102499</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>10</v>
       </c>
@@ -819,8 +880,11 @@
       <c r="F26">
         <v>0.84819999999999995</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26">
+        <v>2.2515296936035099</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>10</v>
       </c>
@@ -839,8 +903,11 @@
       <c r="F27">
         <v>0.84140000000000004</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27">
+        <v>2.53928017616271</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>10</v>
       </c>
@@ -859,8 +926,11 @@
       <c r="F28">
         <v>0.84089999999999998</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28">
+        <v>3.00693535804748</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>10</v>
       </c>
@@ -879,8 +949,11 @@
       <c r="F29">
         <v>0.83750000000000002</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29">
+        <v>3.20503497123718</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>10</v>
       </c>
@@ -899,8 +972,11 @@
       <c r="F30">
         <v>0.83699999999999997</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30">
+        <v>3.2413525581359801</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>15</v>
       </c>
@@ -919,8 +995,11 @@
       <c r="F31">
         <v>0.85050000000000003</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31">
+        <v>2.42216944694519</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>15</v>
       </c>
@@ -939,8 +1018,11 @@
       <c r="F32">
         <v>0.84299999999999997</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32">
+        <v>2.62954521179199</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>15</v>
       </c>
@@ -959,8 +1041,11 @@
       <c r="F33">
         <v>0.84</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33">
+        <v>3.0764145851135201</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>15</v>
       </c>
@@ -979,8 +1064,11 @@
       <c r="F34">
         <v>0.83740000000000003</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34">
+        <v>3.2621762752532901</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>15</v>
       </c>
@@ -999,8 +1087,11 @@
       <c r="F35">
         <v>0.83950000000000002</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35">
+        <v>3.3576793670654199</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>20</v>
       </c>
@@ -1019,8 +1110,11 @@
       <c r="F36">
         <v>0.84489999999999998</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G36">
+        <v>2.2772898674011199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>20</v>
       </c>
@@ -1039,8 +1133,11 @@
       <c r="F37">
         <v>0.83960000000000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G37">
+        <v>2.53040218353271</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>20</v>
       </c>
@@ -1059,8 +1156,11 @@
       <c r="F38">
         <v>0.83879999999999999</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G38">
+        <v>3.01656770706176</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>20</v>
       </c>
@@ -1079,8 +1179,11 @@
       <c r="F39">
         <v>0.83789999999999998</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G39">
+        <v>3.2333617210388099</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>20</v>
       </c>
@@ -1099,8 +1202,11 @@
       <c r="F40">
         <v>0.83950000000000002</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G40">
+        <v>3.3374674320220898</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -1121,12 +1227,12 @@
         <v>0.85229999999999995</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>6</v>
       </c>
@@ -1145,8 +1251,11 @@
       <c r="F44" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G44" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2</v>
       </c>
@@ -1165,8 +1274,11 @@
       <c r="F45">
         <v>0.85389999999999999</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G45">
+        <v>2.22319364547729</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2</v>
       </c>
@@ -1185,8 +1297,11 @@
       <c r="F46">
         <v>0.84489999999999998</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G46">
+        <v>2.5355250835418701</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2</v>
       </c>
@@ -1205,8 +1320,11 @@
       <c r="F47">
         <v>0.84770000000000001</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G47">
+        <v>2.9168329238891602</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2</v>
       </c>
@@ -1225,8 +1343,11 @@
       <c r="F48">
         <v>0.84440000000000004</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G48">
+        <v>3.11917519569396</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2</v>
       </c>
@@ -1245,8 +1366,11 @@
       <c r="F49">
         <v>0.84850000000000003</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G49">
+        <v>3.2285664081573402</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>5</v>
       </c>
@@ -1265,8 +1389,11 @@
       <c r="F50">
         <v>0.85399999999999998</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G50">
+        <v>2.2524616718292201</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>5</v>
       </c>
@@ -1285,8 +1412,11 @@
       <c r="F51">
         <v>0.84370000000000001</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G51">
+        <v>2.5239553451538002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>5</v>
       </c>
@@ -1305,8 +1435,11 @@
       <c r="F52">
         <v>0.8478</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G52">
+        <v>2.9807033538818302</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>5</v>
       </c>
@@ -1325,8 +1458,11 @@
       <c r="F53">
         <v>0.84630000000000005</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G53">
+        <v>3.1898500919342001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>5</v>
       </c>
@@ -1345,8 +1481,11 @@
       <c r="F54">
         <v>0.84240000000000004</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G54">
+        <v>3.3100514411926198</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>10</v>
       </c>
@@ -1365,8 +1504,11 @@
       <c r="F55">
         <v>0.85670000000000002</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G55">
+        <v>2.3551867008209202</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>10</v>
       </c>
@@ -1385,8 +1527,11 @@
       <c r="F56">
         <v>0.84660000000000002</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G56">
+        <v>2.6284763813018799</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>10</v>
       </c>
@@ -1405,8 +1550,11 @@
       <c r="F57">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G57">
+        <v>3.7010183334350502</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>10</v>
       </c>
@@ -1425,8 +1573,11 @@
       <c r="F58">
         <v>0.84540000000000004</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G58">
+        <v>3.5240099430084202</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>10</v>
       </c>
@@ -1445,8 +1596,11 @@
       <c r="F59">
         <v>0.84379999999999999</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G59">
+        <v>3.7263400554656898</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>15</v>
       </c>
@@ -1465,8 +1619,11 @@
       <c r="F60">
         <v>0.8518</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G60">
+        <v>2.42030429840087</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>15</v>
       </c>
@@ -1485,8 +1642,11 @@
       <c r="F61">
         <v>0.8458</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G61">
+        <v>2.6685400009155198</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>15</v>
       </c>
@@ -1505,8 +1665,11 @@
       <c r="F62">
         <v>0.84609999999999996</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G62">
+        <v>3.23163390159606</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>15</v>
       </c>
@@ -1525,8 +1688,11 @@
       <c r="F63">
         <v>0.84660000000000002</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G63">
+        <v>3.39868831634521</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>15</v>
       </c>
@@ -1545,8 +1711,11 @@
       <c r="F64">
         <v>0.84209999999999996</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G64">
+        <v>3.57817530632019</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>20</v>
       </c>
@@ -1565,8 +1734,11 @@
       <c r="F65">
         <v>0.85199999999999998</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G65">
+        <v>2.42678594589233</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>20</v>
       </c>
@@ -1585,8 +1757,11 @@
       <c r="F66">
         <v>0.84899999999999998</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G66">
+        <v>2.6640350818634002</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>20</v>
       </c>
@@ -1605,8 +1780,11 @@
       <c r="F67">
         <v>0.84540000000000004</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G67">
+        <v>3.2496993541717498</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>20</v>
       </c>
@@ -1625,8 +1803,11 @@
       <c r="F68">
         <v>0.84019999999999995</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G68">
+        <v>3.3456442356109601</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>20</v>
       </c>
@@ -1645,8 +1826,11 @@
       <c r="F69">
         <v>0.84460000000000002</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G69">
+        <v>3.6260089874267498</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>10</v>
       </c>
@@ -1675,18 +1859,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDD47EA0-3033-41A0-90B3-E0A599D4A0D9}">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A12" activeCellId="1" sqref="A41 A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1694,7 +1879,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1707,8 +1892,11 @@
       <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C3">
         <v>0.90900000000000003</v>
       </c>
@@ -1721,13 +1909,16 @@
       <c r="F3">
         <v>0.87139999999999995</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>3.6752555370330802</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1744,8 +1935,11 @@
       <c r="F6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1761,8 +1955,11 @@
       <c r="F7">
         <v>0.87290000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>2.7481286525726301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1778,8 +1975,11 @@
       <c r="F8">
         <v>0.86799999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>2.7609055042266801</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10</v>
       </c>
@@ -1795,8 +1995,11 @@
       <c r="F9">
         <v>0.87490000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>2.8145833015441801</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>15</v>
       </c>
@@ -1812,8 +2015,11 @@
       <c r="F10">
         <v>0.871</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>2.86683797836303</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>20</v>
       </c>
@@ -1829,8 +2035,11 @@
       <c r="F11">
         <v>0.87390000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>2.8872032165527299</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1851,12 +2060,12 @@
         <v>0.87490000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -1875,8 +2084,11 @@
       <c r="F15" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1895,8 +2107,11 @@
       <c r="F16">
         <v>0.87470000000000003</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <v>2.9050810337066602</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1915,8 +2130,11 @@
       <c r="F17">
         <v>0.87209999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17">
+        <v>3.18965411186218</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1935,8 +2153,11 @@
       <c r="F18">
         <v>0.87709999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <v>3.6701912879943799</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1955,8 +2176,11 @@
       <c r="F19">
         <v>0.87639999999999996</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <v>3.82998275756835</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1975,8 +2199,11 @@
       <c r="F20">
         <v>0.87790000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20">
+        <v>3.9852373600006099</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>5</v>
       </c>
@@ -1995,8 +2222,11 @@
       <c r="F21">
         <v>0.87609999999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21">
+        <v>2.90738654136657</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>5</v>
       </c>
@@ -2015,8 +2245,11 @@
       <c r="F22">
         <v>0.87370000000000003</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22">
+        <v>3.1761462688446001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>5</v>
       </c>
@@ -2035,8 +2268,11 @@
       <c r="F23">
         <v>0.87229999999999996</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23">
+        <v>3.6591877937316801</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>5</v>
       </c>
@@ -2055,8 +2291,11 @@
       <c r="F24">
         <v>0.87219999999999998</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <v>3.94208335876464</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>5</v>
       </c>
@@ -2075,8 +2314,11 @@
       <c r="F25">
         <v>0.87360000000000004</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <v>3.96868801116943</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>10</v>
       </c>
@@ -2095,8 +2337,11 @@
       <c r="F26">
         <v>0.87690000000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26">
+        <v>2.93149662017822</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>10</v>
       </c>
@@ -2115,8 +2360,11 @@
       <c r="F27">
         <v>0.87329999999999997</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27">
+        <v>3.12639236450195</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>10</v>
       </c>
@@ -2135,8 +2383,11 @@
       <c r="F28">
         <v>0.87549999999999994</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28">
+        <v>3.7272653579711901</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>10</v>
       </c>
@@ -2155,8 +2406,11 @@
       <c r="F29">
         <v>0.87319999999999998</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29">
+        <v>3.8563377857208199</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>10</v>
       </c>
@@ -2175,8 +2429,11 @@
       <c r="F30">
         <v>0.87490000000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30">
+        <v>4.0016703605651802</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>15</v>
       </c>
@@ -2195,8 +2452,11 @@
       <c r="F31">
         <v>0.87529999999999997</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31">
+        <v>2.96314072608947</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>15</v>
       </c>
@@ -2215,8 +2475,11 @@
       <c r="F32">
         <v>0.87390000000000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32">
+        <v>3.2166650295257502</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>15</v>
       </c>
@@ -2235,8 +2498,11 @@
       <c r="F33">
         <v>0.87480000000000002</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33">
+        <v>3.6146378517150799</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>15</v>
       </c>
@@ -2255,8 +2521,11 @@
       <c r="F34">
         <v>0.87170000000000003</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34">
+        <v>3.8957421779632502</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>15</v>
       </c>
@@ -2275,8 +2544,11 @@
       <c r="F35">
         <v>0.874</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35">
+        <v>3.98351526260375</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>20</v>
       </c>
@@ -2295,8 +2567,11 @@
       <c r="F36">
         <v>0.87260000000000004</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G36">
+        <v>2.9373855590820299</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>20</v>
       </c>
@@ -2315,8 +2590,11 @@
       <c r="F37">
         <v>0.87370000000000003</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G37">
+        <v>3.3298089504241899</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>20</v>
       </c>
@@ -2335,8 +2613,11 @@
       <c r="F38">
         <v>0.87580000000000002</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G38">
+        <v>3.67650842666625</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>20</v>
       </c>
@@ -2355,8 +2636,11 @@
       <c r="F39">
         <v>0.874</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G39">
+        <v>3.92282891273498</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>20</v>
       </c>
@@ -2375,8 +2659,11 @@
       <c r="F40">
         <v>0.87450000000000006</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G40">
+        <v>4.0464794635772696</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
@@ -2397,7 +2684,7 @@
         <v>0.87790000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>9</v>
       </c>
@@ -2407,7 +2694,7 @@
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>6</v>
       </c>
@@ -2426,8 +2713,11 @@
       <c r="F44" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G44" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2</v>
       </c>
@@ -2446,8 +2736,11 @@
       <c r="F45">
         <v>0.87160000000000004</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G45">
+        <v>2.94364213943481</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2</v>
       </c>
@@ -2466,8 +2759,11 @@
       <c r="F46">
         <v>0.87109999999999999</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G46">
+        <v>3.1751916408538801</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2</v>
       </c>
@@ -2486,8 +2782,11 @@
       <c r="F47">
         <v>0.87209999999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G47">
+        <v>3.4872701168060298</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2</v>
       </c>
@@ -2506,8 +2805,11 @@
       <c r="F48">
         <v>0.86260000000000003</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G48">
+        <v>3.6953966617584202</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2</v>
       </c>
@@ -2526,8 +2828,11 @@
       <c r="F49">
         <v>0.86750000000000005</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G49">
+        <v>3.8716437816619802</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>5</v>
       </c>
@@ -2546,8 +2851,11 @@
       <c r="F50">
         <v>0.872</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G50">
+        <v>2.9602642059326101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>5</v>
       </c>
@@ -2566,8 +2874,11 @@
       <c r="F51">
         <v>0.8679</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G51">
+        <v>3.2147748470306299</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>5</v>
       </c>
@@ -2586,8 +2897,11 @@
       <c r="F52">
         <v>0.86699999999999999</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G52">
+        <v>3.5683262348175</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>5</v>
       </c>
@@ -2606,8 +2920,11 @@
       <c r="F53">
         <v>0.8679</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G53">
+        <v>3.8283388614654501</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>5</v>
       </c>
@@ -2626,8 +2943,11 @@
       <c r="F54">
         <v>0.86519999999999997</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G54">
+        <v>3.9336979389190598</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>10</v>
       </c>
@@ -2646,8 +2966,11 @@
       <c r="F55">
         <v>0.87009999999999998</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G55">
+        <v>3.06825375556945</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>10</v>
       </c>
@@ -2666,8 +2989,11 @@
       <c r="F56">
         <v>0.86799999999999999</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G56">
+        <v>3.30327868461608</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>10</v>
       </c>
@@ -2686,8 +3012,11 @@
       <c r="F57">
         <v>0.86650000000000005</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G57">
+        <v>3.75938773155212</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>10</v>
       </c>
@@ -2706,8 +3035,11 @@
       <c r="F58">
         <v>0.8619</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G58">
+        <v>3.9681582450866699</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>10</v>
       </c>
@@ -2726,8 +3058,11 @@
       <c r="F59">
         <v>0.8639</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G59">
+        <v>4.1401290893554599</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>15</v>
       </c>
@@ -2746,8 +3081,11 @@
       <c r="F60">
         <v>0.87250000000000005</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G60">
+        <v>3.18718338012695</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>15</v>
       </c>
@@ -2766,8 +3104,11 @@
       <c r="F61">
         <v>0.86839999999999995</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G61">
+        <v>3.3822002410888601</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>15</v>
       </c>
@@ -2786,8 +3127,11 @@
       <c r="F62">
         <v>0.87209999999999999</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G62">
+        <v>3.84398293495178</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>15</v>
       </c>
@@ -2806,8 +3150,11 @@
       <c r="F63">
         <v>0.8619</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G63">
+        <v>4.0623204708099303</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>15</v>
       </c>
@@ -2826,8 +3173,11 @@
       <c r="F64">
         <v>0.86970000000000003</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G64">
+        <v>4.2318158149719203</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>20</v>
       </c>
@@ -2846,8 +3196,11 @@
       <c r="F65">
         <v>0.86829999999999996</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G65">
+        <v>3.1801593303680402</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>20</v>
       </c>
@@ -2866,8 +3219,11 @@
       <c r="F66">
         <v>0.86980000000000002</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G66">
+        <v>3.3566765785217201</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>20</v>
       </c>
@@ -2886,8 +3242,11 @@
       <c r="F67">
         <v>0.86650000000000005</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G67">
+        <v>3.9401898384094198</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>20</v>
       </c>
@@ -2906,8 +3265,11 @@
       <c r="F68">
         <v>0.8639</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G68">
+        <v>4.0665929317474303</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>20</v>
       </c>
@@ -2926,8 +3288,11 @@
       <c r="F69">
         <v>0.86580000000000001</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G69">
+        <v>4.2383651733398402</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>10</v>
       </c>
@@ -2940,7 +3305,7 @@
         <v>0.91020000000000001</v>
       </c>
       <c r="E70">
-        <f t="shared" ref="D70:F70" si="2">MAX(E45:E69)</f>
+        <f t="shared" ref="E70:F70" si="2">MAX(E45:E69)</f>
         <v>0.90780000000000005</v>
       </c>
       <c r="F70">

</xml_diff>

<commit_message>
Added median runtime across 3 runs
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VCU\CMSC635\Project\BorderlineSMOTE-Experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6626CD18-B7DC-4153-85AA-CABEF305839C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C871AD44-884D-46A9-BE50-A72F1965A41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="14">
   <si>
     <t>Unsampled</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Runtime (s)</t>
+  </si>
+  <si>
+    <t>Median Runtime (s)</t>
   </si>
 </sst>
 </file>
@@ -108,9 +111,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,19 +398,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -412,7 +420,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -426,11 +434,16 @@
       <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C3">
         <v>0.88370000000000004</v>
       </c>
@@ -446,8 +459,18 @@
       <c r="G3">
         <v>3.0109384059906001</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <v>3.42527770996093</v>
+      </c>
+      <c r="I3">
+        <v>3.0278677940368599</v>
+      </c>
+      <c r="J3">
+        <f>MEDIAN(G3:I3)</f>
+        <v>3.0278677940368599</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -457,7 +480,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -473,11 +496,13 @@
       <c r="F6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -496,8 +521,18 @@
       <c r="G7">
         <v>2.1193897724151598</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7">
+        <v>2.40770387649536</v>
+      </c>
+      <c r="I7">
+        <v>2.1197409629821702</v>
+      </c>
+      <c r="J7">
+        <f>MEDIAN(G7:I7)</f>
+        <v>2.1197409629821702</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
@@ -516,8 +551,18 @@
       <c r="G8">
         <v>2.0937805175781201</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8">
+        <v>2.2885711193084699</v>
+      </c>
+      <c r="I8">
+        <v>2.1178097724914502</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ref="J8:J11" si="0">MEDIAN(G8:I8)</f>
+        <v>2.1178097724914502</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10</v>
       </c>
@@ -536,8 +581,18 @@
       <c r="G9">
         <v>2.1435699462890598</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9">
+        <v>2.3815045356750399</v>
+      </c>
+      <c r="I9">
+        <v>2.14969277381896</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>2.14969277381896</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>15</v>
       </c>
@@ -556,8 +611,18 @@
       <c r="G10">
         <v>2.162353515625</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10">
+        <v>2.3979110717773402</v>
+      </c>
+      <c r="I10">
+        <v>2.18757104873657</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>2.18757104873657</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>20</v>
       </c>
@@ -576,8 +641,18 @@
       <c r="G11">
         <v>2.22353911399841</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11">
+        <v>2.3003368377685498</v>
+      </c>
+      <c r="I11">
+        <v>2.2584762573242099</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>2.2584762573242099</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -586,19 +661,19 @@
         <v>0.8861</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:F12" si="0">MAX(D7:D11)</f>
+        <f t="shared" ref="D12:F12" si="1">MAX(D7:D11)</f>
         <v>0.89339999999999997</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.88080000000000003</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.84660000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -608,7 +683,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -627,11 +702,16 @@
       <c r="F15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -653,8 +733,18 @@
       <c r="G16">
         <v>2.2552626132964999</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16">
+        <v>2.2890658378600999</v>
+      </c>
+      <c r="I16">
+        <v>2.2407360076904199</v>
+      </c>
+      <c r="J16">
+        <f>MEDIAN(G16:I16)</f>
+        <v>2.2552626132964999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -676,8 +766,18 @@
       <c r="G17">
         <v>2.5098481178283598</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17">
+        <v>2.6804625988006499</v>
+      </c>
+      <c r="I17">
+        <v>2.5292620658874498</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ref="J17:J40" si="2">MEDIAN(G17:I17)</f>
+        <v>2.5292620658874498</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -699,8 +799,18 @@
       <c r="G18">
         <v>2.8897750377654998</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18">
+        <v>2.9762926101684499</v>
+      </c>
+      <c r="I18">
+        <v>2.8665599822997998</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="2"/>
+        <v>2.8897750377654998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -722,8 +832,18 @@
       <c r="G19">
         <v>3.09475350379943</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19">
+        <v>3.2000963687896702</v>
+      </c>
+      <c r="I19">
+        <v>3.1858210563659601</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="2"/>
+        <v>3.1858210563659601</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -745,8 +865,18 @@
       <c r="G20">
         <v>3.2664694786071702</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20">
+        <v>3.2984125614166202</v>
+      </c>
+      <c r="I20">
+        <v>3.2730507850646902</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="2"/>
+        <v>3.2730507850646902</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>5</v>
       </c>
@@ -768,8 +898,18 @@
       <c r="G21">
         <v>2.2354357242584202</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21">
+        <v>2.2613210678100502</v>
+      </c>
+      <c r="I21">
+        <v>2.21721220016479</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="2"/>
+        <v>2.2354357242584202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>5</v>
       </c>
@@ -791,8 +931,18 @@
       <c r="G22">
         <v>2.5341119766235298</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22">
+        <v>2.6429378986358598</v>
+      </c>
+      <c r="I22">
+        <v>2.5456895828246999</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="2"/>
+        <v>2.5456895828246999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>5</v>
       </c>
@@ -814,8 +964,18 @@
       <c r="G23">
         <v>2.9711067676544101</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23">
+        <v>2.9506206512451101</v>
+      </c>
+      <c r="I23">
+        <v>2.9414381980895898</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="2"/>
+        <v>2.9506206512451101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>5</v>
       </c>
@@ -837,8 +997,18 @@
       <c r="G24">
         <v>3.09894371032714</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24">
+        <v>3.1387073993682799</v>
+      </c>
+      <c r="I24">
+        <v>3.0887207984924299</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="2"/>
+        <v>3.09894371032714</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>5</v>
       </c>
@@ -860,8 +1030,18 @@
       <c r="G25">
         <v>3.2883157730102499</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25">
+        <v>3.2897284030914302</v>
+      </c>
+      <c r="I25">
+        <v>3.18212890625</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="2"/>
+        <v>3.2883157730102499</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>10</v>
       </c>
@@ -883,8 +1063,18 @@
       <c r="G26">
         <v>2.2515296936035099</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H26">
+        <v>2.2568664550781201</v>
+      </c>
+      <c r="I26">
+        <v>2.28619289398193</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="2"/>
+        <v>2.2568664550781201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>10</v>
       </c>
@@ -906,8 +1096,18 @@
       <c r="G27">
         <v>2.53928017616271</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H27">
+        <v>2.6681933403015101</v>
+      </c>
+      <c r="I27">
+        <v>2.6178882122039702</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="2"/>
+        <v>2.6178882122039702</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>10</v>
       </c>
@@ -929,8 +1129,18 @@
       <c r="G28">
         <v>3.00693535804748</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H28">
+        <v>2.9792931079864502</v>
+      </c>
+      <c r="I28">
+        <v>2.9830517768859801</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="2"/>
+        <v>2.9830517768859801</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>10</v>
       </c>
@@ -952,8 +1162,18 @@
       <c r="G29">
         <v>3.20503497123718</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H29">
+        <v>3.19071316719055</v>
+      </c>
+      <c r="I29">
+        <v>3.2601971626281698</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="2"/>
+        <v>3.20503497123718</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>10</v>
       </c>
@@ -975,8 +1195,18 @@
       <c r="G30">
         <v>3.2413525581359801</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H30">
+        <v>3.3255448341369598</v>
+      </c>
+      <c r="I30">
+        <v>3.2586894035339302</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="2"/>
+        <v>3.2586894035339302</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>15</v>
       </c>
@@ -998,8 +1228,18 @@
       <c r="G31">
         <v>2.42216944694519</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H31">
+        <v>2.2483382225036599</v>
+      </c>
+      <c r="I31">
+        <v>2.3152291774749698</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="2"/>
+        <v>2.3152291774749698</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>15</v>
       </c>
@@ -1021,8 +1261,18 @@
       <c r="G32">
         <v>2.62954521179199</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H32">
+        <v>2.7038824558257999</v>
+      </c>
+      <c r="I32">
+        <v>2.6208548545837398</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="2"/>
+        <v>2.62954521179199</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>15</v>
       </c>
@@ -1044,8 +1294,18 @@
       <c r="G33">
         <v>3.0764145851135201</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H33">
+        <v>2.9956128597259499</v>
+      </c>
+      <c r="I33">
+        <v>3.0419108867645201</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="2"/>
+        <v>3.0419108867645201</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>15</v>
       </c>
@@ -1067,8 +1327,18 @@
       <c r="G34">
         <v>3.2621762752532901</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H34">
+        <v>3.1658074855804399</v>
+      </c>
+      <c r="I34">
+        <v>3.16613268852233</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="2"/>
+        <v>3.16613268852233</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>15</v>
       </c>
@@ -1090,8 +1360,18 @@
       <c r="G35">
         <v>3.3576793670654199</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H35">
+        <v>3.3414251804351802</v>
+      </c>
+      <c r="I35">
+        <v>3.2941033840179399</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="2"/>
+        <v>3.3414251804351802</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>20</v>
       </c>
@@ -1113,8 +1393,18 @@
       <c r="G36">
         <v>2.2772898674011199</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H36">
+        <v>2.33941555023193</v>
+      </c>
+      <c r="I36">
+        <v>2.3368227481842001</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="2"/>
+        <v>2.3368227481842001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>20</v>
       </c>
@@ -1136,8 +1426,18 @@
       <c r="G37">
         <v>2.53040218353271</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H37">
+        <v>2.6428740024566602</v>
+      </c>
+      <c r="I37">
+        <v>2.6520938873290998</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="2"/>
+        <v>2.6428740024566602</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>20</v>
       </c>
@@ -1159,8 +1459,18 @@
       <c r="G38">
         <v>3.01656770706176</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H38">
+        <v>3.0562648773193302</v>
+      </c>
+      <c r="I38">
+        <v>3.0019245147704998</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="2"/>
+        <v>3.01656770706176</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>20</v>
       </c>
@@ -1182,8 +1492,18 @@
       <c r="G39">
         <v>3.2333617210388099</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H39">
+        <v>3.23986315727233</v>
+      </c>
+      <c r="I39">
+        <v>3.1941044330596902</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="2"/>
+        <v>3.2333617210388099</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>20</v>
       </c>
@@ -1205,8 +1525,18 @@
       <c r="G40">
         <v>3.3374674320220898</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H40">
+        <v>3.3843817710876398</v>
+      </c>
+      <c r="I40">
+        <v>3.3227584362029998</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="2"/>
+        <v>3.3374674320220898</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -1215,24 +1545,24 @@
         <v>0.89119999999999999</v>
       </c>
       <c r="D41">
-        <f t="shared" ref="D41:F41" si="1">MAX(D16:D40)</f>
+        <f t="shared" ref="D41:F41" si="3">MAX(D16:D40)</f>
         <v>0.89659999999999995</v>
       </c>
       <c r="E41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.8871</v>
       </c>
       <c r="F41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.85229999999999995</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>6</v>
       </c>
@@ -1251,11 +1581,16 @@
       <c r="F44" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="G44" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2</v>
       </c>
@@ -1277,8 +1612,18 @@
       <c r="G45">
         <v>2.22319364547729</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H45">
+        <v>2.27286171913146</v>
+      </c>
+      <c r="I45">
+        <v>2.2265369892120299</v>
+      </c>
+      <c r="J45">
+        <f t="shared" ref="J45:J69" si="4">MEDIAN(G45:I45)</f>
+        <v>2.2265369892120299</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2</v>
       </c>
@@ -1300,8 +1645,18 @@
       <c r="G46">
         <v>2.5355250835418701</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H46">
+        <v>2.5534708499908398</v>
+      </c>
+      <c r="I46">
+        <v>2.5375936031341499</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="4"/>
+        <v>2.5375936031341499</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2</v>
       </c>
@@ -1323,8 +1678,18 @@
       <c r="G47">
         <v>2.9168329238891602</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H47">
+        <v>2.9968123435974099</v>
+      </c>
+      <c r="I47">
+        <v>2.93417000770568</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="4"/>
+        <v>2.93417000770568</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2</v>
       </c>
@@ -1346,8 +1711,18 @@
       <c r="G48">
         <v>3.11917519569396</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H48">
+        <v>3.1811151504516602</v>
+      </c>
+      <c r="I48">
+        <v>3.0874443054199201</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="4"/>
+        <v>3.11917519569396</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2</v>
       </c>
@@ -1369,8 +1744,18 @@
       <c r="G49">
         <v>3.2285664081573402</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H49">
+        <v>3.2627902030944802</v>
+      </c>
+      <c r="I49">
+        <v>3.2049045562744101</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="4"/>
+        <v>3.2285664081573402</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>5</v>
       </c>
@@ -1392,8 +1777,18 @@
       <c r="G50">
         <v>2.2524616718292201</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H50">
+        <v>2.30168533325195</v>
+      </c>
+      <c r="I50">
+        <v>2.2693967819213801</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="4"/>
+        <v>2.2693967819213801</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>5</v>
       </c>
@@ -1415,8 +1810,18 @@
       <c r="G51">
         <v>2.5239553451538002</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H51">
+        <v>2.5954201221465998</v>
+      </c>
+      <c r="I51">
+        <v>2.5412456989288299</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="4"/>
+        <v>2.5412456989288299</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>5</v>
       </c>
@@ -1438,8 +1843,18 @@
       <c r="G52">
         <v>2.9807033538818302</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H52">
+        <v>3.0116913318634002</v>
+      </c>
+      <c r="I52">
+        <v>3.0038282871246298</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="4"/>
+        <v>3.0038282871246298</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>5</v>
       </c>
@@ -1461,8 +1876,18 @@
       <c r="G53">
         <v>3.1898500919342001</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H53">
+        <v>3.1247189044952299</v>
+      </c>
+      <c r="I53">
+        <v>3.2667062282562198</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="4"/>
+        <v>3.1898500919342001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>5</v>
       </c>
@@ -1484,8 +1909,18 @@
       <c r="G54">
         <v>3.3100514411926198</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H54">
+        <v>3.3107109069824201</v>
+      </c>
+      <c r="I54">
+        <v>3.2655558586120601</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="4"/>
+        <v>3.3100514411926198</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>10</v>
       </c>
@@ -1507,8 +1942,18 @@
       <c r="G55">
         <v>2.3551867008209202</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H55">
+        <v>2.4354877471923801</v>
+      </c>
+      <c r="I55">
+        <v>2.44364142417907</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="4"/>
+        <v>2.4354877471923801</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>10</v>
       </c>
@@ -1530,8 +1975,18 @@
       <c r="G56">
         <v>2.6284763813018799</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H56">
+        <v>2.6681542396545401</v>
+      </c>
+      <c r="I56">
+        <v>2.67106962203979</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="4"/>
+        <v>2.6681542396545401</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>10</v>
       </c>
@@ -1553,8 +2008,18 @@
       <c r="G57">
         <v>3.7010183334350502</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H57">
+        <v>3.1582932472228999</v>
+      </c>
+      <c r="I57">
+        <v>3.0917255878448402</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="4"/>
+        <v>3.1582932472228999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>10</v>
       </c>
@@ -1576,8 +2041,18 @@
       <c r="G58">
         <v>3.5240099430084202</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H58">
+        <v>3.3230957984924299</v>
+      </c>
+      <c r="I58">
+        <v>3.3066341876983598</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="4"/>
+        <v>3.3230957984924299</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>10</v>
       </c>
@@ -1599,8 +2074,18 @@
       <c r="G59">
         <v>3.7263400554656898</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H59">
+        <v>3.5178544521331698</v>
+      </c>
+      <c r="I59">
+        <v>3.4850881099700901</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="4"/>
+        <v>3.5178544521331698</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>15</v>
       </c>
@@ -1622,8 +2107,18 @@
       <c r="G60">
         <v>2.42030429840087</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H60">
+        <v>2.4378814697265598</v>
+      </c>
+      <c r="I60">
+        <v>2.4117224216461102</v>
+      </c>
+      <c r="J60">
+        <f t="shared" si="4"/>
+        <v>2.42030429840087</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>15</v>
       </c>
@@ -1645,8 +2140,18 @@
       <c r="G61">
         <v>2.6685400009155198</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H61">
+        <v>2.8999683856964098</v>
+      </c>
+      <c r="I61">
+        <v>2.7072296142578098</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="4"/>
+        <v>2.7072296142578098</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>15</v>
       </c>
@@ -1668,8 +2173,18 @@
       <c r="G62">
         <v>3.23163390159606</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H62">
+        <v>3.1463313102722101</v>
+      </c>
+      <c r="I62">
+        <v>3.1643211841583199</v>
+      </c>
+      <c r="J62">
+        <f t="shared" si="4"/>
+        <v>3.1643211841583199</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>15</v>
       </c>
@@ -1691,8 +2206,18 @@
       <c r="G63">
         <v>3.39868831634521</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H63">
+        <v>3.4489927291870099</v>
+      </c>
+      <c r="I63">
+        <v>3.3426551818847599</v>
+      </c>
+      <c r="J63">
+        <f t="shared" si="4"/>
+        <v>3.39868831634521</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>15</v>
       </c>
@@ -1714,8 +2239,18 @@
       <c r="G64">
         <v>3.57817530632019</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H64">
+        <v>3.5449855327606201</v>
+      </c>
+      <c r="I64">
+        <v>3.5312054157257</v>
+      </c>
+      <c r="J64">
+        <f t="shared" si="4"/>
+        <v>3.5449855327606201</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>20</v>
       </c>
@@ -1737,8 +2272,18 @@
       <c r="G65">
         <v>2.42678594589233</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H65">
+        <v>2.4923675060272199</v>
+      </c>
+      <c r="I65">
+        <v>2.4267277717590301</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="4"/>
+        <v>2.42678594589233</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>20</v>
       </c>
@@ -1760,8 +2305,18 @@
       <c r="G66">
         <v>2.6640350818634002</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H66">
+        <v>2.75725889205932</v>
+      </c>
+      <c r="I66">
+        <v>2.6621921062469398</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="4"/>
+        <v>2.6640350818634002</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>20</v>
       </c>
@@ -1783,8 +2338,18 @@
       <c r="G67">
         <v>3.2496993541717498</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H67">
+        <v>3.1858246326446502</v>
+      </c>
+      <c r="I67">
+        <v>3.2027134895324698</v>
+      </c>
+      <c r="J67">
+        <f t="shared" si="4"/>
+        <v>3.2027134895324698</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>20</v>
       </c>
@@ -1806,8 +2371,18 @@
       <c r="G68">
         <v>3.3456442356109601</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H68">
+        <v>3.4783587455749498</v>
+      </c>
+      <c r="I68">
+        <v>3.4080576896667401</v>
+      </c>
+      <c r="J68">
+        <f t="shared" si="4"/>
+        <v>3.4080576896667401</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>20</v>
       </c>
@@ -1829,8 +2404,18 @@
       <c r="G69">
         <v>3.6260089874267498</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H69">
+        <v>3.61005640029907</v>
+      </c>
+      <c r="I69">
+        <v>3.54352450370788</v>
+      </c>
+      <c r="J69">
+        <f t="shared" si="4"/>
+        <v>3.61005640029907</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>10</v>
       </c>
@@ -1839,39 +2424,49 @@
         <v>0.89449999999999996</v>
       </c>
       <c r="D70">
-        <f t="shared" ref="D70:F70" si="2">MAX(D45:D69)</f>
+        <f t="shared" ref="D70:F70" si="5">MAX(D45:D69)</f>
         <v>0.89959999999999996</v>
       </c>
       <c r="E70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.89059999999999995</v>
       </c>
       <c r="F70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.85670000000000002</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G2:I2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="J7 J3" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDD47EA0-3033-41A0-90B3-E0A599D4A0D9}">
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="N62" sqref="N62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1879,7 +2474,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1892,11 +2487,16 @@
       <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C3">
         <v>0.90900000000000003</v>
       </c>
@@ -1912,13 +2512,23 @@
       <c r="G3">
         <v>3.6752555370330802</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <v>3.6533112525939901</v>
+      </c>
+      <c r="I3">
+        <v>3.6640145778656001</v>
+      </c>
+      <c r="J3">
+        <f>MEDIAN(G3:I3)</f>
+        <v>3.6640145778656001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1938,8 +2548,11 @@
       <c r="G6" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1958,8 +2571,18 @@
       <c r="G7">
         <v>2.7481286525726301</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7">
+        <v>2.7301979064941402</v>
+      </c>
+      <c r="I7">
+        <v>2.7600924968719398</v>
+      </c>
+      <c r="J7">
+        <f>MEDIAN(G7:I7)</f>
+        <v>2.7481286525726301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1978,8 +2601,18 @@
       <c r="G8">
         <v>2.7609055042266801</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8">
+        <v>2.7839550971984801</v>
+      </c>
+      <c r="I8">
+        <v>2.8382527828216499</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ref="J8:J11" si="0">MEDIAN(G8:I8)</f>
+        <v>2.7839550971984801</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10</v>
       </c>
@@ -1998,8 +2631,18 @@
       <c r="G9">
         <v>2.8145833015441801</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9">
+        <v>2.8314445018768302</v>
+      </c>
+      <c r="I9">
+        <v>2.8123848438262899</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>2.8145833015441801</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>15</v>
       </c>
@@ -2018,8 +2661,18 @@
       <c r="G10">
         <v>2.86683797836303</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10">
+        <v>2.8734204769134499</v>
+      </c>
+      <c r="I10">
+        <v>2.8739364147186199</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>2.8734204769134499</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>20</v>
       </c>
@@ -2038,8 +2691,18 @@
       <c r="G11">
         <v>2.8872032165527299</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11">
+        <v>2.8512115478515598</v>
+      </c>
+      <c r="I11">
+        <v>2.86264896392822</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>2.86264896392822</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2048,24 +2711,24 @@
         <v>0.90980000000000005</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:F12" si="0">MAX(D7:D11)</f>
+        <f t="shared" ref="D12:F12" si="1">MAX(D7:D11)</f>
         <v>0.91159999999999997</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.90839999999999999</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.87490000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -2084,11 +2747,16 @@
       <c r="F15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2110,8 +2778,18 @@
       <c r="G16">
         <v>2.9050810337066602</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16">
+        <v>2.84419465065002</v>
+      </c>
+      <c r="I16">
+        <v>2.8674137592315598</v>
+      </c>
+      <c r="J16">
+        <f>MEDIAN(G16:I16)</f>
+        <v>2.8674137592315598</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2133,8 +2811,18 @@
       <c r="G17">
         <v>3.18965411186218</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17">
+        <v>3.1750683784484801</v>
+      </c>
+      <c r="I17">
+        <v>3.2847087383270201</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ref="J17:J40" si="2">MEDIAN(G17:I17)</f>
+        <v>3.18965411186218</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2156,8 +2844,18 @@
       <c r="G18">
         <v>3.6701912879943799</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18">
+        <v>3.6265404224395699</v>
+      </c>
+      <c r="I18">
+        <v>3.7174398899078298</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="2"/>
+        <v>3.6701912879943799</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2179,8 +2877,18 @@
       <c r="G19">
         <v>3.82998275756835</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19">
+        <v>3.86865901947021</v>
+      </c>
+      <c r="I19">
+        <v>3.8680467605590798</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="2"/>
+        <v>3.8680467605590798</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2202,8 +2910,18 @@
       <c r="G20">
         <v>3.9852373600006099</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20">
+        <v>3.9874851703643799</v>
+      </c>
+      <c r="I20">
+        <v>4.0196130275726301</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="2"/>
+        <v>3.9874851703643799</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>5</v>
       </c>
@@ -2225,8 +2943,18 @@
       <c r="G21">
         <v>2.90738654136657</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21">
+        <v>2.9397375583648602</v>
+      </c>
+      <c r="I21">
+        <v>2.9208993911743102</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="2"/>
+        <v>2.9208993911743102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>5</v>
       </c>
@@ -2248,8 +2976,18 @@
       <c r="G22">
         <v>3.1761462688446001</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22">
+        <v>3.27702665328979</v>
+      </c>
+      <c r="I22">
+        <v>3.2490420341491699</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="2"/>
+        <v>3.2490420341491699</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>5</v>
       </c>
@@ -2271,8 +3009,18 @@
       <c r="G23">
         <v>3.6591877937316801</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23">
+        <v>3.6849954128265301</v>
+      </c>
+      <c r="I23">
+        <v>3.6540052890777499</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="2"/>
+        <v>3.6591877937316801</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>5</v>
       </c>
@@ -2294,8 +3042,18 @@
       <c r="G24">
         <v>3.94208335876464</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24">
+        <v>3.83795142173767</v>
+      </c>
+      <c r="I24">
+        <v>3.89938187599182</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="2"/>
+        <v>3.89938187599182</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>5</v>
       </c>
@@ -2317,8 +3075,18 @@
       <c r="G25">
         <v>3.96868801116943</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25">
+        <v>4.0484130382537797</v>
+      </c>
+      <c r="I25">
+        <v>4.0086166858673096</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="2"/>
+        <v>4.0086166858673096</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>10</v>
       </c>
@@ -2340,8 +3108,18 @@
       <c r="G26">
         <v>2.93149662017822</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H26">
+        <v>2.9473781585693302</v>
+      </c>
+      <c r="I26">
+        <v>2.9511363506317099</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="2"/>
+        <v>2.9473781585693302</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>10</v>
       </c>
@@ -2363,8 +3141,18 @@
       <c r="G27">
         <v>3.12639236450195</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H27">
+        <v>3.2396669387817298</v>
+      </c>
+      <c r="I27">
+        <v>3.11509704589843</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="2"/>
+        <v>3.12639236450195</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>10</v>
       </c>
@@ -2386,8 +3174,18 @@
       <c r="G28">
         <v>3.7272653579711901</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H28">
+        <v>3.5934367179870601</v>
+      </c>
+      <c r="I28">
+        <v>3.6563014984130802</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="2"/>
+        <v>3.6563014984130802</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>10</v>
       </c>
@@ -2409,8 +3207,18 @@
       <c r="G29">
         <v>3.8563377857208199</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H29">
+        <v>3.9100821018218901</v>
+      </c>
+      <c r="I29">
+        <v>3.9248032569885201</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="2"/>
+        <v>3.9100821018218901</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>10</v>
       </c>
@@ -2432,8 +3240,18 @@
       <c r="G30">
         <v>4.0016703605651802</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H30">
+        <v>3.9719376564025799</v>
+      </c>
+      <c r="I30">
+        <v>3.9569578170776301</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="2"/>
+        <v>3.9719376564025799</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>15</v>
       </c>
@@ -2455,8 +3273,18 @@
       <c r="G31">
         <v>2.96314072608947</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H31">
+        <v>2.9642710685729901</v>
+      </c>
+      <c r="I31">
+        <v>3.00227451324462</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="2"/>
+        <v>2.9642710685729901</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>15</v>
       </c>
@@ -2478,8 +3306,18 @@
       <c r="G32">
         <v>3.2166650295257502</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H32">
+        <v>3.3197281360626198</v>
+      </c>
+      <c r="I32">
+        <v>3.27846026420593</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="2"/>
+        <v>3.27846026420593</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>15</v>
       </c>
@@ -2501,8 +3339,18 @@
       <c r="G33">
         <v>3.6146378517150799</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H33">
+        <v>3.6078829765319802</v>
+      </c>
+      <c r="I33">
+        <v>3.7378742694854701</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="2"/>
+        <v>3.6146378517150799</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>15</v>
       </c>
@@ -2524,8 +3372,18 @@
       <c r="G34">
         <v>3.8957421779632502</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H34">
+        <v>3.8381567001342698</v>
+      </c>
+      <c r="I34">
+        <v>3.9341778755187899</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="2"/>
+        <v>3.8957421779632502</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>15</v>
       </c>
@@ -2547,8 +3405,18 @@
       <c r="G35">
         <v>3.98351526260375</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H35">
+        <v>3.9977889060974099</v>
+      </c>
+      <c r="I35">
+        <v>4.1501111984252903</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="2"/>
+        <v>3.9977889060974099</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>20</v>
       </c>
@@ -2570,8 +3438,18 @@
       <c r="G36">
         <v>2.9373855590820299</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H36">
+        <v>2.9471571445464999</v>
+      </c>
+      <c r="I36">
+        <v>2.9665992259979199</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="2"/>
+        <v>2.9471571445464999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>20</v>
       </c>
@@ -2593,8 +3471,18 @@
       <c r="G37">
         <v>3.3298089504241899</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H37">
+        <v>3.2303569316864</v>
+      </c>
+      <c r="I37">
+        <v>3.27514123916625</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="2"/>
+        <v>3.27514123916625</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>20</v>
       </c>
@@ -2616,8 +3504,18 @@
       <c r="G38">
         <v>3.67650842666625</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H38">
+        <v>3.7200007438659601</v>
+      </c>
+      <c r="I38">
+        <v>3.6907107830047599</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="2"/>
+        <v>3.6907107830047599</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>20</v>
       </c>
@@ -2639,8 +3537,18 @@
       <c r="G39">
         <v>3.92282891273498</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H39">
+        <v>3.9151363372802699</v>
+      </c>
+      <c r="I39">
+        <v>3.99022269248962</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="2"/>
+        <v>3.92282891273498</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>20</v>
       </c>
@@ -2662,8 +3570,18 @@
       <c r="G40">
         <v>4.0464794635772696</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H40">
+        <v>4.0128459930419904</v>
+      </c>
+      <c r="I40">
+        <v>3.9905867576599099</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="2"/>
+        <v>4.0128459930419904</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
@@ -2672,19 +3590,19 @@
         <v>0.91390000000000005</v>
       </c>
       <c r="D41">
-        <f t="shared" ref="D41:F41" si="1">MAX(D16:D40)</f>
+        <f t="shared" ref="D41:F41" si="3">MAX(D16:D40)</f>
         <v>0.91469999999999996</v>
       </c>
       <c r="E41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.9133</v>
       </c>
       <c r="F41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.87790000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>9</v>
       </c>
@@ -2694,7 +3612,7 @@
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>6</v>
       </c>
@@ -2713,11 +3631,16 @@
       <c r="F44" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="G44" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2</v>
       </c>
@@ -2739,8 +3662,18 @@
       <c r="G45">
         <v>2.94364213943481</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H45">
+        <v>2.85839319229125</v>
+      </c>
+      <c r="I45">
+        <v>2.95041728019714</v>
+      </c>
+      <c r="J45">
+        <f>MEDIAN(G45:I45)</f>
+        <v>2.94364213943481</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2</v>
       </c>
@@ -2762,8 +3695,18 @@
       <c r="G46">
         <v>3.1751916408538801</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H46">
+        <v>3.1202590465545601</v>
+      </c>
+      <c r="I46">
+        <v>3.0883595943450901</v>
+      </c>
+      <c r="J46">
+        <f t="shared" ref="J46:J69" si="4">MEDIAN(G46:I46)</f>
+        <v>3.1202590465545601</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2</v>
       </c>
@@ -2785,8 +3728,18 @@
       <c r="G47">
         <v>3.4872701168060298</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H47">
+        <v>3.5513458251953098</v>
+      </c>
+      <c r="I47">
+        <v>3.51385450363159</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="4"/>
+        <v>3.51385450363159</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2</v>
       </c>
@@ -2808,8 +3761,18 @@
       <c r="G48">
         <v>3.6953966617584202</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H48">
+        <v>3.7249877452850302</v>
+      </c>
+      <c r="I48">
+        <v>3.8178439140319802</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="4"/>
+        <v>3.7249877452850302</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2</v>
       </c>
@@ -2831,8 +3794,18 @@
       <c r="G49">
         <v>3.8716437816619802</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H49">
+        <v>3.8656075000762899</v>
+      </c>
+      <c r="I49">
+        <v>3.79038405418396</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="4"/>
+        <v>3.8656075000762899</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>5</v>
       </c>
@@ -2854,8 +3827,18 @@
       <c r="G50">
         <v>2.9602642059326101</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H50">
+        <v>2.95177102088928</v>
+      </c>
+      <c r="I50">
+        <v>2.9738535881042401</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="4"/>
+        <v>2.9602642059326101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>5</v>
       </c>
@@ -2877,8 +3860,18 @@
       <c r="G51">
         <v>3.2147748470306299</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H51">
+        <v>3.2222335338592498</v>
+      </c>
+      <c r="I51">
+        <v>3.1942389011382999</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="4"/>
+        <v>3.2147748470306299</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>5</v>
       </c>
@@ -2900,8 +3893,18 @@
       <c r="G52">
         <v>3.5683262348175</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H52">
+        <v>3.6832015514373699</v>
+      </c>
+      <c r="I52">
+        <v>3.66303086280822</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="4"/>
+        <v>3.66303086280822</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>5</v>
       </c>
@@ -2923,8 +3926,18 @@
       <c r="G53">
         <v>3.8283388614654501</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H53">
+        <v>3.8080406188964799</v>
+      </c>
+      <c r="I53">
+        <v>3.8177304267883301</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="4"/>
+        <v>3.8177304267883301</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>5</v>
       </c>
@@ -2946,8 +3959,18 @@
       <c r="G54">
         <v>3.9336979389190598</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H54">
+        <v>3.9725387096404998</v>
+      </c>
+      <c r="I54">
+        <v>3.9581775665283199</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="4"/>
+        <v>3.9581775665283199</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>10</v>
       </c>
@@ -2969,8 +3992,18 @@
       <c r="G55">
         <v>3.06825375556945</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H55">
+        <v>3.1022820472717201</v>
+      </c>
+      <c r="I55">
+        <v>3.1746747493743799</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="4"/>
+        <v>3.1022820472717201</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>10</v>
       </c>
@@ -2992,8 +4025,18 @@
       <c r="G56">
         <v>3.30327868461608</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H56">
+        <v>3.3873414993286102</v>
+      </c>
+      <c r="I56">
+        <v>3.2610023021697998</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="4"/>
+        <v>3.30327868461608</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>10</v>
       </c>
@@ -3015,8 +4058,18 @@
       <c r="G57">
         <v>3.75938773155212</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H57">
+        <v>3.81458067893981</v>
+      </c>
+      <c r="I57">
+        <v>3.7761917114257799</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="4"/>
+        <v>3.7761917114257799</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>10</v>
       </c>
@@ -3038,8 +4091,18 @@
       <c r="G58">
         <v>3.9681582450866699</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H58">
+        <v>3.98837041854858</v>
+      </c>
+      <c r="I58">
+        <v>3.9628262519836399</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="4"/>
+        <v>3.9681582450866699</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>10</v>
       </c>
@@ -3061,8 +4124,18 @@
       <c r="G59">
         <v>4.1401290893554599</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H59">
+        <v>4.1570107936859104</v>
+      </c>
+      <c r="I59">
+        <v>4.0661818981170601</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="4"/>
+        <v>4.1401290893554599</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>15</v>
       </c>
@@ -3084,8 +4157,18 @@
       <c r="G60">
         <v>3.18718338012695</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H60">
+        <v>3.2402431964874201</v>
+      </c>
+      <c r="I60">
+        <v>3.1863973140716499</v>
+      </c>
+      <c r="J60">
+        <f t="shared" si="4"/>
+        <v>3.18718338012695</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>15</v>
       </c>
@@ -3107,8 +4190,18 @@
       <c r="G61">
         <v>3.3822002410888601</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H61">
+        <v>3.4079403877258301</v>
+      </c>
+      <c r="I61">
+        <v>3.3916392326354901</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="4"/>
+        <v>3.3916392326354901</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>15</v>
       </c>
@@ -3130,8 +4223,18 @@
       <c r="G62">
         <v>3.84398293495178</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H62">
+        <v>3.9505774974822998</v>
+      </c>
+      <c r="I62">
+        <v>3.8923926353454501</v>
+      </c>
+      <c r="J62">
+        <f t="shared" si="4"/>
+        <v>3.8923926353454501</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>15</v>
       </c>
@@ -3153,8 +4256,18 @@
       <c r="G63">
         <v>4.0623204708099303</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H63">
+        <v>4.0394256114959699</v>
+      </c>
+      <c r="I63">
+        <v>4.0505254268646196</v>
+      </c>
+      <c r="J63">
+        <f t="shared" si="4"/>
+        <v>4.0505254268646196</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>15</v>
       </c>
@@ -3176,8 +4289,18 @@
       <c r="G64">
         <v>4.2318158149719203</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H64">
+        <v>4.2002110481262198</v>
+      </c>
+      <c r="I64">
+        <v>4.2069075107574401</v>
+      </c>
+      <c r="J64">
+        <f t="shared" si="4"/>
+        <v>4.2069075107574401</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>20</v>
       </c>
@@ -3199,8 +4322,18 @@
       <c r="G65">
         <v>3.1801593303680402</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H65">
+        <v>3.1779918670654199</v>
+      </c>
+      <c r="I65">
+        <v>3.1779944896697998</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="4"/>
+        <v>3.1779944896697998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>20</v>
       </c>
@@ -3222,8 +4355,18 @@
       <c r="G66">
         <v>3.3566765785217201</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H66">
+        <v>3.39665603637695</v>
+      </c>
+      <c r="I66">
+        <v>3.38714575767517</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="4"/>
+        <v>3.38714575767517</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>20</v>
       </c>
@@ -3245,8 +4388,18 @@
       <c r="G67">
         <v>3.9401898384094198</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H67">
+        <v>3.9308989048004102</v>
+      </c>
+      <c r="I67">
+        <v>3.9086666107177699</v>
+      </c>
+      <c r="J67">
+        <f t="shared" si="4"/>
+        <v>3.9308989048004102</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>20</v>
       </c>
@@ -3268,8 +4421,18 @@
       <c r="G68">
         <v>4.0665929317474303</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H68">
+        <v>4.0776271820068297</v>
+      </c>
+      <c r="I68">
+        <v>4.1034059524536097</v>
+      </c>
+      <c r="J68">
+        <f t="shared" si="4"/>
+        <v>4.0776271820068297</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>20</v>
       </c>
@@ -3291,8 +4454,18 @@
       <c r="G69">
         <v>4.2383651733398402</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H69">
+        <v>4.2954025268554599</v>
+      </c>
+      <c r="I69">
+        <v>4.2174949645995996</v>
+      </c>
+      <c r="J69">
+        <f t="shared" si="4"/>
+        <v>4.2383651733398402</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>10</v>
       </c>
@@ -3305,15 +4478,20 @@
         <v>0.91020000000000001</v>
       </c>
       <c r="E70">
-        <f t="shared" ref="E70:F70" si="2">MAX(E45:E69)</f>
+        <f t="shared" ref="E70:F70" si="5">MAX(E45:E69)</f>
         <v>0.90780000000000005</v>
       </c>
       <c r="F70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.87250000000000005</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G44:I44"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>